<commit_message>
Added full correlation analysis and summary statistics
</commit_message>
<xml_diff>
--- a/vix_vstoxx_results.xlsx
+++ b/vix_vstoxx_results.xlsx
@@ -520,8 +520,12 @@
       <c r="D3" t="n">
         <v>0</v>
       </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
+      <c r="E3" t="n">
+        <v>31</v>
+      </c>
+      <c r="F3" t="n">
+        <v>4424</v>
+      </c>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr">
         <is>
@@ -706,14 +710,24 @@
       <c r="B2" t="n">
         <v>12</v>
       </c>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
+      <c r="C2" t="n">
+        <v>718.6642156973709</v>
+      </c>
+      <c r="D2" t="n">
+        <v>4.450569524860884e-146</v>
+      </c>
+      <c r="E2" t="n">
+        <v>71.32817042295778</v>
+      </c>
+      <c r="F2" t="n">
+        <v>7.333424758267242e-160</v>
+      </c>
+      <c r="G2" t="n">
+        <v>4425</v>
+      </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Cannot reject no-ARCH</t>
+          <t>Reject no-ARCH (vol clustering)</t>
         </is>
       </c>
     </row>
@@ -803,7 +817,11 @@
       <c r="H2" t="n">
         <v>3.666646766025368</v>
       </c>
-      <c r="I2" t="inlineStr"/>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Standardized Student's t</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -922,7 +940,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -933,10 +951,35 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>n_obs</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>mse</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>mae</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>directional_hits</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>directional_hit_rate</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>window</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>ar_order_p</t>
         </is>
@@ -947,9 +990,24 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
+        <v>1409</v>
+      </c>
+      <c r="C2" t="n">
+        <v>13.22533602837114</v>
+      </c>
+      <c r="D2" t="n">
+        <v>2.009767936038296</v>
+      </c>
+      <c r="E2" t="n">
+        <v>830</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.5894886363636364</v>
+      </c>
+      <c r="G2" t="n">
         <v>90</v>
       </c>
-      <c r="C2" t="n">
+      <c r="H2" t="n">
         <v>6</v>
       </c>
     </row>

</xml_diff>